<commit_message>
Julkinen data ja viimeinen
</commit_message>
<xml_diff>
--- a/inst/ennustekuvat/ptt_ennusteet_KT_2022_1.xlsx
+++ b/inst/ennustekuvat/ptt_ennusteet_KT_2022_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pttry-my.sharepoint.com/personal/janne_huovari_ptt_fi/Documents/Rpkg/pttrobo/inst/ennustekuvat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{83310B53-87FB-406E-B32B-C5F152F2F3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84D98803-204F-487A-9D23-C58B2721FB69}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{83310B53-87FB-406E-B32B-C5F152F2F3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F82F4285-B3B6-4F63-9377-DE685912052C}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="2070" windowWidth="19155" windowHeight="12480" xr2:uid="{064C7390-CFFB-4D1E-AC46-6ACB68398C33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{064C7390-CFFB-4D1E-AC46-6ACB68398C33}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>BKT</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Nettoluotonanto Jukinen sektori</t>
+  </si>
+  <si>
+    <t>Velkasuhde</t>
   </si>
 </sst>
 </file>
@@ -306,7 +309,7 @@
             <v>4.6786592549834648E-3</v>
           </cell>
           <cell r="M5">
-            <v>9.6762377273743906E-3</v>
+            <v>1.0445423191837461E-2</v>
           </cell>
         </row>
         <row r="6">
@@ -466,7 +469,7 @@
             <v>4.6780091416962488E-3</v>
           </cell>
           <cell r="M12">
-            <v>-1.7986551045387489E-2</v>
+            <v>-1.7887045416287717E-2</v>
           </cell>
         </row>
         <row r="13">
@@ -536,6 +539,7 @@
       </sheetData>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
+      <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -652,6 +656,11 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
+        <row r="11">
+          <cell r="D11">
+            <v>4.9773755656108642E-2</v>
+          </cell>
+        </row>
         <row r="20">
           <cell r="D20">
             <v>2651</v>
@@ -845,7 +854,12 @@
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
@@ -900,106 +914,138 @@
             <v>-3.2039978808701082E-2</v>
           </cell>
           <cell r="L4">
-            <v>-1.4990842595399328E-2</v>
+            <v>-1.7112896638108534E-2</v>
           </cell>
           <cell r="M4">
-            <v>9.5326172914270545E-3</v>
+            <v>-2.0272503245166142E-2</v>
           </cell>
         </row>
         <row r="5">
           <cell r="D5">
-            <v>-6.9938181800606103E-3</v>
+            <v>-7.3176508117565745E-3</v>
           </cell>
           <cell r="E5">
-            <v>-7.1622868226222294E-3</v>
+            <v>-6.2492608274002416E-3</v>
           </cell>
           <cell r="F5">
-            <v>-6.0730606202705067E-3</v>
+            <v>-4.1283939719931224E-3</v>
           </cell>
           <cell r="G5">
-            <v>-3.9681662917972083E-3</v>
+            <v>-1.997339826160733E-3</v>
           </cell>
           <cell r="H5">
-            <v>-1.9360254938578306E-3</v>
+            <v>-8.7420974180615757E-3</v>
           </cell>
           <cell r="I5">
-            <v>-8.5094141387188765E-3</v>
+            <v>-1.2528559278221571E-2</v>
           </cell>
           <cell r="J5">
-            <v>-1.2563289144729931E-2</v>
+            <v>-5.0421227336708751E-4</v>
           </cell>
           <cell r="K5">
-            <v>1.8186562502471002E-4</v>
+            <v>-3.3368388591490271E-3</v>
           </cell>
           <cell r="L5">
-            <v>-4.1444425376250334E-4</v>
+            <v>-2.2817195517478043E-3</v>
           </cell>
           <cell r="M5">
-            <v>-1.0001913297691657E-2</v>
+            <v>-5.5288645214089478E-3</v>
           </cell>
         </row>
         <row r="6">
           <cell r="D6">
-            <v>1.8530959849586994E-2</v>
+            <v>1.4809301246513966E-2</v>
           </cell>
           <cell r="E6">
-            <v>1.4494879012228871E-2</v>
+            <v>1.1831492300778202E-2</v>
           </cell>
           <cell r="F6">
-            <v>1.1497899024448551E-2</v>
+            <v>1.3410384427955387E-2</v>
           </cell>
           <cell r="G6">
-            <v>1.2889912108209863E-2</v>
+            <v>1.3305288089756563E-2</v>
           </cell>
           <cell r="H6">
-            <v>1.2896842393818424E-2</v>
+            <v>1.2789761337742218E-2</v>
           </cell>
           <cell r="I6">
-            <v>1.2449343761986559E-2</v>
+            <v>1.3891900005003085E-2</v>
           </cell>
           <cell r="J6">
-            <v>1.3991890585936679E-2</v>
+            <v>3.9076451185949282E-4</v>
           </cell>
           <cell r="K6">
-            <v>4.1512805712162065E-4</v>
+            <v>9.5637597159733377E-3</v>
           </cell>
           <cell r="L6">
-            <v>7.6847587878483229E-3</v>
+            <v>1.4450890494402761E-2</v>
           </cell>
           <cell r="M6">
-            <v>1.2100483410756233E-2</v>
+            <v>1.1057729042817896E-2</v>
           </cell>
         </row>
         <row r="7">
           <cell r="D7">
-            <v>-2.5829277369899033E-2</v>
+            <v>-2.9874768604668023E-2</v>
           </cell>
           <cell r="E7">
-            <v>-2.2503961965134708E-2</v>
+            <v>-2.4254322681363388E-2</v>
           </cell>
           <cell r="F7">
-            <v>-2.0839654649270404E-2</v>
+            <v>-1.6982502597486186E-2</v>
           </cell>
           <cell r="G7">
-            <v>-8.9261647098333643E-3</v>
+            <v>-6.539962262650187E-3</v>
           </cell>
           <cell r="H7">
-            <v>-1.6190655678722566E-3</v>
+            <v>-8.5322185481522088E-3</v>
           </cell>
           <cell r="I7">
-            <v>-6.8834114370528495E-3</v>
+            <v>-9.4600003335390155E-3</v>
           </cell>
           <cell r="J7">
-            <v>-5.3568352276308323E-2</v>
+            <v>-5.5110401479022665E-2</v>
           </cell>
           <cell r="K7">
-            <v>-3.1442985126554752E-2</v>
+            <v>-2.5813057951876776E-2</v>
           </cell>
           <cell r="L7">
-            <v>-7.720528061313508E-3</v>
+            <v>-4.9437256954535762E-3</v>
           </cell>
           <cell r="M7">
-            <v>1.1631187404491629E-2</v>
+            <v>-1.4743638723757193E-2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="D17">
+            <v>0.59825961710416287</v>
+          </cell>
+          <cell r="E17">
+            <v>0.63641696430683348</v>
+          </cell>
+          <cell r="F17">
+            <v>0.63176380805266685</v>
+          </cell>
+          <cell r="G17">
+            <v>0.61167206508146232</v>
+          </cell>
+          <cell r="H17">
+            <v>0.5977864204087926</v>
+          </cell>
+          <cell r="I17">
+            <v>0.5959424978736888</v>
+          </cell>
+          <cell r="J17">
+            <v>0.68985482888295968</v>
+          </cell>
+          <cell r="K17">
+            <v>0.65792262013015257</v>
+          </cell>
+          <cell r="L17">
+            <v>0.65185305014107153</v>
+          </cell>
+          <cell r="M17">
+            <v>0.6539209224051219</v>
           </cell>
         </row>
       </sheetData>
@@ -1313,19 +1359,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7F8266-A289-4E7B-843E-FBDDAD3BAAD2}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="2" width="27.44140625" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1379,7 +1425,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1430,10 +1476,10 @@
       </c>
       <c r="N2">
         <f>100* '[1]Huoltotase, iterointi'!M5</f>
-        <v>0.96762377273743905</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.0445423191837462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1487,7 +1533,7 @@
         <v>3.5000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1541,7 +1587,7 @@
         <v>3.5000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1595,7 +1641,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1649,7 +1695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1700,10 +1746,10 @@
       </c>
       <c r="N7">
         <f>100* '[1]Huoltotase, iterointi'!M12</f>
-        <v>-1.7986551045387489</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>-1.7887045416287717</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1757,7 +1803,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1811,7 +1857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1824,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1837,7 +1883,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1888,7 +1934,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1901,7 +1947,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1914,7 +1960,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1927,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1940,7 +1986,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1991,7 +2037,7 @@
         <v>73.452822009796421</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -2042,7 +2088,7 @@
         <v>7.1752744819401943</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2093,7 +2139,7 @@
         <v>2790.8939999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2144,7 +2190,7 @@
         <v>2590.6396949999998</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D21" s="3" t="s">
         <v>37</v>
       </c>
@@ -2189,7 +2235,7 @@
         <v>2.4730600000000038</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D22" s="3" t="s">
         <v>38</v>
       </c>
@@ -2227,146 +2273,191 @@
       </c>
       <c r="M22">
         <f>100*'[5]Syöttö Julk.tasapaino'!L4</f>
-        <v>-1.4990842595399327</v>
+        <v>-1.7112896638108535</v>
       </c>
       <c r="N22">
         <f>100*'[5]Syöttö Julk.tasapaino'!M4</f>
-        <v>0.95326172914270546</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>-2.027250324516614</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D23" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E23">
         <f>100*'[5]Syöttö Julk.tasapaino'!D5</f>
-        <v>-0.69938181800606103</v>
+        <v>-0.73176508117565742</v>
       </c>
       <c r="F23">
         <f>100*'[5]Syöttö Julk.tasapaino'!E5</f>
-        <v>-0.71622868226222292</v>
+        <v>-0.62492608274002415</v>
       </c>
       <c r="G23">
         <f>100*'[5]Syöttö Julk.tasapaino'!F5</f>
-        <v>-0.60730606202705073</v>
+        <v>-0.41283939719931223</v>
       </c>
       <c r="H23">
         <f>100*'[5]Syöttö Julk.tasapaino'!G5</f>
-        <v>-0.39681662917972083</v>
+        <v>-0.19973398261607331</v>
       </c>
       <c r="I23">
         <f>100*'[5]Syöttö Julk.tasapaino'!H5</f>
-        <v>-0.19360254938578306</v>
+        <v>-0.87420974180615763</v>
       </c>
       <c r="J23">
         <f>100*'[5]Syöttö Julk.tasapaino'!I5</f>
-        <v>-0.8509414138718876</v>
+        <v>-1.2528559278221572</v>
       </c>
       <c r="K23">
         <f>100*'[5]Syöttö Julk.tasapaino'!J5</f>
-        <v>-1.2563289144729932</v>
+        <v>-5.042122733670875E-2</v>
       </c>
       <c r="L23">
         <f>100*'[5]Syöttö Julk.tasapaino'!K5</f>
-        <v>1.8186562502471002E-2</v>
+        <v>-0.33368388591490272</v>
       </c>
       <c r="M23">
         <f>100*'[5]Syöttö Julk.tasapaino'!L5</f>
-        <v>-4.1444425376250336E-2</v>
+        <v>-0.22817195517478042</v>
       </c>
       <c r="N23">
         <f>100*'[5]Syöttö Julk.tasapaino'!M5</f>
-        <v>-1.0001913297691658</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>-0.55288645214089482</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E24">
         <f>100*'[5]Syöttö Julk.tasapaino'!D6</f>
-        <v>1.8530959849586994</v>
+        <v>1.4809301246513966</v>
       </c>
       <c r="F24">
         <f>100*'[5]Syöttö Julk.tasapaino'!E6</f>
-        <v>1.4494879012228872</v>
+        <v>1.1831492300778201</v>
       </c>
       <c r="G24">
         <f>100*'[5]Syöttö Julk.tasapaino'!F6</f>
-        <v>1.1497899024448552</v>
+        <v>1.3410384427955386</v>
       </c>
       <c r="H24">
         <f>100*'[5]Syöttö Julk.tasapaino'!G6</f>
-        <v>1.2889912108209862</v>
+        <v>1.3305288089756564</v>
       </c>
       <c r="I24">
         <f>100*'[5]Syöttö Julk.tasapaino'!H6</f>
-        <v>1.2896842393818424</v>
+        <v>1.2789761337742218</v>
       </c>
       <c r="J24">
         <f>100*'[5]Syöttö Julk.tasapaino'!I6</f>
-        <v>1.244934376198656</v>
+        <v>1.3891900005003086</v>
       </c>
       <c r="K24">
         <f>100*'[5]Syöttö Julk.tasapaino'!J6</f>
-        <v>1.3991890585936679</v>
+        <v>3.9076451185949282E-2</v>
       </c>
       <c r="L24">
         <f>100*'[5]Syöttö Julk.tasapaino'!K6</f>
-        <v>4.1512805712162065E-2</v>
+        <v>0.95637597159733378</v>
       </c>
       <c r="M24">
         <f>100*'[5]Syöttö Julk.tasapaino'!L6</f>
-        <v>0.76847587878483226</v>
+        <v>1.4450890494402762</v>
       </c>
       <c r="N24">
         <f>100*'[5]Syöttö Julk.tasapaino'!M6</f>
-        <v>1.2100483410756233</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.1057729042817896</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D25" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E25">
         <f>100*'[5]Syöttö Julk.tasapaino'!D7</f>
-        <v>-2.5829277369899031</v>
+        <v>-2.9874768604668023</v>
       </c>
       <c r="F25">
         <f>100*'[5]Syöttö Julk.tasapaino'!E7</f>
-        <v>-2.2503961965134707</v>
+        <v>-2.4254322681363387</v>
       </c>
       <c r="G25">
         <f>100*'[5]Syöttö Julk.tasapaino'!F7</f>
-        <v>-2.0839654649270405</v>
+        <v>-1.6982502597486187</v>
       </c>
       <c r="H25">
         <f>100*'[5]Syöttö Julk.tasapaino'!G7</f>
-        <v>-0.89261647098333641</v>
+        <v>-0.65399622626501874</v>
       </c>
       <c r="I25">
         <f>100*'[5]Syöttö Julk.tasapaino'!H7</f>
-        <v>-0.16190655678722565</v>
+        <v>-0.85322185481522084</v>
       </c>
       <c r="J25">
         <f>100*'[5]Syöttö Julk.tasapaino'!I7</f>
-        <v>-0.68834114370528499</v>
+        <v>-0.94600003335390159</v>
       </c>
       <c r="K25">
         <f>100*'[5]Syöttö Julk.tasapaino'!J7</f>
-        <v>-5.3568352276308326</v>
+        <v>-5.5110401479022668</v>
       </c>
       <c r="L25">
         <f>100*'[5]Syöttö Julk.tasapaino'!K7</f>
-        <v>-3.1442985126554754</v>
+        <v>-2.5813057951876774</v>
       </c>
       <c r="M25">
         <f>100*'[5]Syöttö Julk.tasapaino'!L7</f>
-        <v>-0.77205280613135085</v>
+        <v>-0.49437256954535763</v>
       </c>
       <c r="N25">
         <f>100*'[5]Syöttö Julk.tasapaino'!M7</f>
-        <v>1.163118740449163</v>
+        <v>-1.4743638723757193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!D17</f>
+        <v>59.825961710416287</v>
+      </c>
+      <c r="F26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!E17</f>
+        <v>63.641696430683346</v>
+      </c>
+      <c r="G26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!F17</f>
+        <v>63.176380805266689</v>
+      </c>
+      <c r="H26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!G17</f>
+        <v>61.167206508146229</v>
+      </c>
+      <c r="I26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!H17</f>
+        <v>59.778642040879262</v>
+      </c>
+      <c r="J26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!I17</f>
+        <v>59.594249787368881</v>
+      </c>
+      <c r="K26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!J17</f>
+        <v>68.985482888295962</v>
+      </c>
+      <c r="L26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!K17</f>
+        <v>65.792262013015261</v>
+      </c>
+      <c r="M26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!L17</f>
+        <v>65.185305014107158</v>
+      </c>
+      <c r="N26">
+        <f>100*'[5]Syöttö Julk.tasapaino'!M17</f>
+        <v>65.392092240512184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>